<commit_message>
V3: -Correciones de errores -Agregado de comentarios -Arreglo de nombres de actividades -Modularizaciones de actividades
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kpaz-my.sharepoint.com/personal/diego_ramirez_kpaz_cl/Documents/Documentos/UiPath/RPA_EDSA_ChallengeFinal/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="291" documentId="13_ncr:1_{75BA7D11-E0E2-4DB6-B19C-105A7EA0FE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B04352B-D798-4EA7-B16A-3019001F6808}"/>
+  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{75BA7D11-E0E2-4DB6-B19C-105A7EA0FE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A932530-6EA1-4382-A734-679414EC629F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-1935" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,90 @@
   </si>
   <si>
     <t>ProcessABCQueue</t>
+  </si>
+  <si>
+    <t>ProcessFullName</t>
+  </si>
+  <si>
+    <t>ProcessShortName</t>
+  </si>
+  <si>
+    <t>Lista de procesos necesarios para la ejecucion limpia del RPA</t>
+  </si>
+  <si>
+    <t>Lista corta de procesos necesarios para la ejecucion limpia del RPA</t>
+  </si>
+  <si>
+    <t>msedge,excel</t>
+  </si>
+  <si>
+    <t>System.Diagnostics.Process (msedge),System.Diagnostics.Process (EXCEL)</t>
+  </si>
+  <si>
+    <t>UrlAmazon</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/</t>
+  </si>
+  <si>
+    <t>Pagina de Amazon la cual se debe realizar las busquedas de articulos</t>
+  </si>
+  <si>
+    <t>SpamTimeOut</t>
+  </si>
+  <si>
+    <t>LenguajeTrabajo</t>
+  </si>
+  <si>
+    <t>MonedaTrabajo</t>
+  </si>
+  <si>
+    <t>Se define la moneda que debe tener los precios de los productos de Amazon</t>
+  </si>
+  <si>
+    <t>FileDatosAmazon</t>
+  </si>
+  <si>
+    <t>Data\Input\datos_buscar.xlsx</t>
+  </si>
+  <si>
+    <t>Ruta del archivo de Amazon con los productos a buscar</t>
+  </si>
+  <si>
+    <t>SheetName</t>
+  </si>
+  <si>
+    <t>Productos</t>
+  </si>
+  <si>
+    <t>Nombre Hoja de productos de Amazon</t>
+  </si>
+  <si>
+    <t>CLP - Chilean Peso</t>
+  </si>
+  <si>
+    <t>Se define el idioma que debe tener la pagina de Amazon al momento de trabajar English - EN</t>
+  </si>
+  <si>
+    <t>English - EN</t>
+  </si>
+  <si>
+    <t>FileOutputDatos</t>
+  </si>
+  <si>
+    <t>Data\Input\TemplateOutput.xlsx</t>
+  </si>
+  <si>
+    <t>GitHubRepo</t>
+  </si>
+  <si>
+    <t>https://github.com/DiegoRPATssr/RPA_EDSA_DR</t>
+  </si>
+  <si>
+    <t>Repositorio donde se almacena el proyecto en GitHub</t>
+  </si>
+  <si>
+    <t>Ruta de archivo informe del proceso</t>
   </si>
 </sst>
 </file>
@@ -218,14 +302,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -242,6 +326,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,54 +630,54 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="71.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="129.1796875" style="3" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" style="3" customWidth="1"/>
-    <col min="27" max="16384" width="14.453125" style="3"/>
+    <col min="1" max="1" width="32.54296875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="65" style="4" customWidth="1"/>
+    <col min="3" max="3" width="94.453125" style="4" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" style="4" customWidth="1"/>
+    <col min="27" max="16384" width="14.453125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.5">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="5" t="s">
@@ -611,15 +699,125 @@
         <v>32</v>
       </c>
     </row>
+    <row r="4" spans="1:26" ht="29">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
+      <c r="A5" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
+      <c r="A13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -685,7 +883,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>25</v>
@@ -2850,26 +3048,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="10d2cc5f-9b3f-43f2-b8dc-169dcd64a43b" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee1c9b29-7680-41d1-b5d5-edf00f3d0f8d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010002630800BD558B4DAD2D6511683E4CDA" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="f6f6be082771558f0f16c2835f0ded95">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee1c9b29-7680-41d1-b5d5-edf00f3d0f8d" xmlns:ns3="10d2cc5f-9b3f-43f2-b8dc-169dcd64a43b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5763d397a48ee2fe3c4161db0e58c35" ns2:_="" ns3:_="">
     <xsd:import namespace="ee1c9b29-7680-41d1-b5d5-edf00f3d0f8d"/>
@@ -3118,26 +3296,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81840DF6-A240-4919-AF69-24F6ADF8A182}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="10d2cc5f-9b3f-43f2-b8dc-169dcd64a43b"/>
-    <ds:schemaRef ds:uri="ee1c9b29-7680-41d1-b5d5-edf00f3d0f8d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA34861F-A3E7-450C-815D-1965460CF712}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="10d2cc5f-9b3f-43f2-b8dc-169dcd64a43b" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ee1c9b29-7680-41d1-b5d5-edf00f3d0f8d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC7C30E0-4716-4FD1-B512-548443273FCA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3154,4 +3333,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA34861F-A3E7-450C-815D-1965460CF712}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81840DF6-A240-4919-AF69-24F6ADF8A182}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="10d2cc5f-9b3f-43f2-b8dc-169dcd64a43b"/>
+    <ds:schemaRef ds:uri="ee1c9b29-7680-41d1-b5d5-edf00f3d0f8d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
V4: -Correciones de errores -Agregado de comentarios -Arreglo de nombres de actividades -Modularizaciones de actividades -Agregado Notificacion de Correo en formato HTML -Actualizacion de GitHub y inclusion de GitHub en correo HTML
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kpaz-my.sharepoint.com/personal/diego_ramirez_kpaz_cl/Documents/Documentos/UiPath/RPA_EDSA_ChallengeFinal/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="368" documentId="13_ncr:1_{75BA7D11-E0E2-4DB6-B19C-105A7EA0FE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A932530-6EA1-4382-A734-679414EC629F}"/>
+  <xr:revisionPtr revIDLastSave="419" documentId="13_ncr:1_{75BA7D11-E0E2-4DB6-B19C-105A7EA0FE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24CB8D5E-5A46-4CBE-AB2D-CF687D9E5E4C}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1935" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -244,6 +244,122 @@
   </si>
   <si>
     <t>Ruta de archivo informe del proceso</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html lang="es"&gt;
+&lt;head&gt;
+    &lt;meta charset="UTF-8"&gt;
+    &lt;title&gt;Notificación de Ejecución de Proceso&lt;/title&gt;
+&lt;/head&gt;
+&lt;body style="font-family: Arial, sans-serif; line-height: 1.6; color: #333;"&gt;
+    &lt;h2 style="color: #007bff;"&gt;Ejecución del proceso {0} ha finalizado correctamente.&lt;/h2&gt;
+    &lt;p&gt;
+        &lt;strong&gt;Hora de inicio:&lt;/strong&gt; {1}&lt;br&gt;
+        &lt;strong&gt;Hora de Finalización:&lt;/strong&gt; {2}&lt;br&gt;
+        &lt;strong&gt;Usuario Robot Ejecutante:&lt;/strong&gt; {3}&lt;br&gt;
+        &lt;strong&gt;Zona horaria de ejecución del Robot:&lt;/strong&gt; {4}&lt;br&gt;
+        &lt;strong&gt;Máquina de ejecución del Robot:&lt;/strong&gt; {5}
+    &lt;/p&gt;
+    &lt;p style="margin-top: 20px;"&gt;
+        &lt;strong&gt;Información adicional:&lt;/strong&gt;&lt;br&gt;
+        &lt;a href="{6}" style="color: #007bff; text-decoration: none;"&gt;Enlace GitHub del Proyecto&lt;/a&gt;
+    &lt;/p&gt;
+    &lt;p style="font-style: italic; color: #666;"&gt;
+        Notificación generada por "{7}"
+    &lt;/p&gt;
+    &lt;p&gt;Se despide, &lt;br&gt;
+       Robot {0}&lt;br&gt;
+       Asistido por &lt;br&gt;
+       Diego Ramirez Rojas&lt;br&gt;
+       Desarrollador RPA UiPath - VBA - Python
+    &lt;/p&gt;
+&lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Body con formato de HTML para envio de notificacion del Robot</t>
+  </si>
+  <si>
+    <t>equipo_rpa@edsa.com.ar</t>
+  </si>
+  <si>
+    <t>Destinatarios del Robot</t>
+  </si>
+  <si>
+    <t>Notifi_From</t>
+  </si>
+  <si>
+    <t>CC_From</t>
+  </si>
+  <si>
+    <t>diego.ramirez@kpaz.cl</t>
+  </si>
+  <si>
+    <t>El proceso {0} ha finalizado correctamente a las {1}</t>
+  </si>
+  <si>
+    <t>SubjectFinishedOk</t>
+  </si>
+  <si>
+    <t>SubjectFinishedError</t>
+  </si>
+  <si>
+    <t>El proceso {0} ha finalizado con un error de ejecucion a las {1}</t>
+  </si>
+  <si>
+    <t>Usuario Con copia que recibira el correo</t>
+  </si>
+  <si>
+    <t>Asunto con notificacion de error de ejecucion</t>
+  </si>
+  <si>
+    <t>Asunto con notificacion exitosa de ejecucion</t>
+  </si>
+  <si>
+    <t>BodyHTMLOK</t>
+  </si>
+  <si>
+    <t>BodyHTMLError</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html lang="es"&gt;
+&lt;head&gt;
+    &lt;meta charset="UTF-8"&gt;
+    &lt;title&gt;Notificación de Ejecución de Proceso&lt;/title&gt;
+&lt;/head&gt;
+&lt;body style="font-family: Arial, sans-serif; line-height: 1.6; color: #333;"&gt;
+    &lt;h2 style="color: #007bff;"&gt;Ejecución del proceso {0} ha finalizado con una excepción.&lt;/h2&gt;
+    &lt;p style="color: #ff0000; font-weight: bold;"&gt;
+        Detalles de la excepción que finalizó la ejecución:&lt;br&gt;
+        {8}
+    &lt;/p&gt;
+    &lt;p&gt;
+        &lt;strong&gt;Hora de inicio:&lt;/strong&gt; {1}&lt;br&gt;
+        &lt;strong&gt;Hora de Finalización:&lt;/strong&gt; {2}&lt;br&gt;
+        &lt;strong&gt;Usuario Robot Ejecutante:&lt;/strong&gt; {3}&lt;br&gt;
+        &lt;strong&gt;Zona horaria de ejecución del Robot:&lt;/strong&gt; {4}&lt;br&gt;
+        &lt;strong&gt;Máquina de ejecución del Robot:&lt;/strong&gt; {5}
+    &lt;/p&gt;
+    &lt;p style="margin-top: 20px;"&gt;
+        &lt;strong&gt;Información adicional:&lt;/strong&gt;&lt;br&gt;
+        &lt;a href="{6}" style="color: #007bff; text-decoration: none;"&gt;Enlace GitHub del Proyecto&lt;/a&gt;
+    &lt;/p&gt;
+    &lt;p style="font-style: italic; color: #666;"&gt;
+        Notificación generada por "{7}"
+    &lt;/p&gt;
+    &lt;p&gt;Se despide, &lt;br&gt;
+       Robot {0}&lt;br&gt;
+       Asistido por &lt;br&gt;
+       Diego Ramirez Rojas&lt;br&gt;
+       Desarrollador RPA UiPath - VBA - Python
+    &lt;/p&gt;
+&lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>Body con formato de HTML para envio de notificacion del Robot pero con excepcion incluida</t>
   </si>
 </sst>
 </file>
@@ -296,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -311,6 +427,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +750,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -813,11 +933,77 @@
       <c r="A14" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="409.5">
+      <c r="A19" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="409.5">
+      <c r="A20" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>